<commit_message>
promo plan with date
</commit_message>
<xml_diff>
--- a/static/upload/generate_promoplan_template.xlsx
+++ b/static/upload/generate_promoplan_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C239FA0-11EA-432D-BCB6-4E5C11827811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9131D96F-6188-4FAB-85F4-9BAF2B8D08CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{035C29D6-5D1D-44E5-A1BA-F7D031A3F514}"/>
   </bookViews>
@@ -402,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA74A78-BD77-41EA-8586-16786E18C582}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -443,6 +443,11 @@
         <v>4</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2105500225</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>